<commit_message>
Integrate test data report
</commit_message>
<xml_diff>
--- a/Deliverable 6/Test Data/Test Data Report.xlsx
+++ b/Deliverable 6/Test Data/Test Data Report.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>No.</t>
   </si>
@@ -48,6 +48,181 @@
   </si>
   <si>
     <t>Sad Path</t>
+  </si>
+  <si>
+    <t>Get Provider directory</t>
+  </si>
+  <si>
+    <t>Cheng Luo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click "get all services" button </t>
+  </si>
+  <si>
+    <t>Show service table</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Get member service report for a member</t>
+  </si>
+  <si>
+    <t>show member report</t>
+  </si>
+  <si>
+    <t>11111 / empty</t>
+  </si>
+  <si>
+    <t>Member is null / no result</t>
+  </si>
+  <si>
+    <t>Get Account payable report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click "Get PayableReport" button </t>
+  </si>
+  <si>
+    <t>show account payable report</t>
+  </si>
+  <si>
+    <t>Get provider info</t>
+  </si>
+  <si>
+    <t>Show provider information</t>
+  </si>
+  <si>
+    <t>empty / 11111</t>
+  </si>
+  <si>
+    <t>error message</t>
+  </si>
+  <si>
+    <t>Authenticate member ID</t>
+  </si>
+  <si>
+    <t>1001 / 1006 / 1008</t>
+  </si>
+  <si>
+    <t>vaild / suspended / invaild</t>
+  </si>
+  <si>
+    <t>error message / member not found</t>
+  </si>
+  <si>
+    <t>Update Provider Report Scheduler</t>
+  </si>
+  <si>
+    <t>Time: 12:00AM
+Weekday: Tuesday
+Report Type: Provider Report</t>
+  </si>
+  <si>
+    <t>Success Alert
+Schedule Updated in DB</t>
+  </si>
+  <si>
+    <t>N/A: GUI Constriction</t>
+  </si>
+  <si>
+    <t>Update Member Info</t>
+  </si>
+  <si>
+    <t>ID: 1010
+name: Don Cheadle
+address: 112 25 St South
+city: St. Cloud
+state: MN
+zip: 24123
+status: valid</t>
+  </si>
+  <si>
+    <t>Success Alert
+Member Updated in DB</t>
+  </si>
+  <si>
+    <t>ID: 2000
+ID: 1010
+name: 123X
+city: S12
+state: mn
+zip: 2
+status: valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error Alert
+Error Alert:
+</t>
+  </si>
+  <si>
+    <t>Delete Provider Info</t>
+  </si>
+  <si>
+    <t>ID: 104</t>
+  </si>
+  <si>
+    <t>Success Alert
+Provider Deleted in DB</t>
+  </si>
+  <si>
+    <t>ID: 2000</t>
+  </si>
+  <si>
+    <t>Error Alert</t>
+  </si>
+  <si>
+    <t>Verify Weekly Provider Report Services</t>
+  </si>
+  <si>
+    <t>Provider Login ID: 100
+start date: 11/01/2014
+end date: 12/09/2014</t>
+  </si>
+  <si>
+    <t>Success Alert</t>
+  </si>
+  <si>
+    <t>Provider Login ID: 100
+start date: 09/01/2014
+end date: 10/1/2014</t>
+  </si>
+  <si>
+    <t>Error Alert
+No service record</t>
+  </si>
+  <si>
+    <t>Authenticate Provider</t>
+  </si>
+  <si>
+    <t>Role: Provider
+ID: 100</t>
+  </si>
+  <si>
+    <t>Move to provider area</t>
+  </si>
+  <si>
+    <t>Role: Provider
+ID: 2000</t>
+  </si>
+  <si>
+    <t>Add Service</t>
+  </si>
+  <si>
+    <t>Service Time: Test Service
+Service Code: 200002
+Service Fee: 59.99</t>
+  </si>
+  <si>
+    <t>Success Alert
+Service Added in DB</t>
+  </si>
+  <si>
+    <t>Service Time: Test Service
+Service Code: 100002
+Service Fee: 59.99</t>
+  </si>
+  <si>
+    <t>Edward Iskandar</t>
   </si>
 </sst>
 </file>
@@ -109,15 +284,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -129,6 +298,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -410,23 +594,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="5"/>
+    <col min="1" max="1" width="8.7265625" style="3"/>
     <col min="2" max="2" width="35.08984375" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="6" width="26.1796875" customWidth="1"/>
     <col min="7" max="7" width="26.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="4"/>
+      <c r="A1" s="2"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="6" t="s">
@@ -439,7 +623,7 @@
       <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -448,21 +632,242 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1000</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="9">
+        <v>100</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:G8"/>
+  <autoFilter ref="A2:G8">
+    <sortState ref="A3:G13">
+      <sortCondition ref="B2:B8"/>
+    </sortState>
+  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>

</xml_diff>

<commit_message>
Updated test data report
</commit_message>
<xml_diff>
--- a/Deliverable 6/Test Data/Test Data Report.xlsx
+++ b/Deliverable 6/Test Data/Test Data Report.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="83">
   <si>
     <t>No.</t>
   </si>
@@ -223,6 +223,191 @@
   </si>
   <si>
     <t>Edward Iskandar</t>
+  </si>
+  <si>
+    <t>Update member schedule</t>
+  </si>
+  <si>
+    <t>Shengti Pan</t>
+  </si>
+  <si>
+    <t>8:13:00 PM/ Tuesday /Member Report (The current time: 8:12 PM)</t>
+  </si>
+  <si>
+    <t>8:15:00 PM/ Tuesday /Member Report (The current time: 8:16 PM)</t>
+  </si>
+  <si>
+    <t>no result</t>
+  </si>
+  <si>
+    <t>Update provider schedule</t>
+  </si>
+  <si>
+    <t>8:22:00 PM/ Tuesday /Provider Report (The current time: 8:21 PM)</t>
+  </si>
+  <si>
+    <t>8:24:00 PM/ Tuesday /Member Report (The current time: 8:23 PM)</t>
+  </si>
+  <si>
+    <t>Update EFT schedule</t>
+  </si>
+  <si>
+    <t>8:25:00 PM/ Tuesday /EFT Report (The current time: 8:24 PM)</t>
+  </si>
+  <si>
+    <t>EFT_20_25.txt</t>
+  </si>
+  <si>
+    <t>8:37:00 PM/ Tuesday /EFT Report (The current time: 8:36 PM)</t>
+  </si>
+  <si>
+    <t>Update Account Payable schedule</t>
+  </si>
+  <si>
+    <t>8:27:00 PM/ Tuesday /Account Payable Report (The current time: 8:26 PM)</t>
+  </si>
+  <si>
+    <t>Account_Payable_20_27.txt</t>
+  </si>
+  <si>
+    <t>8:39:00 PM/ Tuesday /Account Payable Report (The current time: 8:38 PM)</t>
+  </si>
+  <si>
+    <t>Get Member Report By Member Id</t>
+  </si>
+  <si>
+    <t>Report Result:
+----------------------Member Report-------------------- 
+Member ID: 1000
+Member Name: Brian Babylon
+State: IL
+Street Address: 21 Jump Street
+Zipcode: 25322
+Status: Invalid
+Service:1
+Service Name: 1 On 1 Consultation
+Service Code: 100001
+Service Fee: 150.00
+-------------------------------</t>
+  </si>
+  <si>
+    <t>member is null</t>
+  </si>
+  <si>
+    <t>Get Provider Report By Provider Id</t>
+  </si>
+  <si>
+    <t>Report Result:
+----------------------Provider Report--------------------
+Provider ID: 100
+Provider Name: Pizza, Health, and You
+City: Washington D.C
+State: WA
+Street Address: 121 20th St South
+Zip Code: 00002
+Service:1
+Service Name: 1 On 1 Consultation
+Service Code: 100001
+Service Fee: 150.00
+-------------------------------
+Service:2
+Service Name: Self Help Books Lib
+Service Code: 100005
+Service Fee: 39.99
+-------------------------------
+Service:3
+Service Name: 1 On 1 Consultation
+Service Code: 100001
+Service Fee: 150.00
+-------------------------------
+Service:4
+Service Name: Group Consultation
+Service Code: 100002
+Service Fee: 50.00
+-------------------------------</t>
+  </si>
+  <si>
+    <t>provider is null</t>
+  </si>
+  <si>
+    <t>Get EFT Report(from webpage)</t>
+  </si>
+  <si>
+    <t>Report Result:
+----------------------EFT Report--------------------
+Bank account: 1231231231
+The total fee: 389.99
+-------------------------------
+Bank account: 3213213211
+The total fee: 0
+-------------------------------
+Bank account: 1112223334
+The total fee: 0
+-------------------------------
+Bank account: 1112223334
+The total fee: 0
+-------------------------------
+Bank account: 1112223334
+The total fee: 0
+-------------------------------</t>
+  </si>
+  <si>
+    <t>Get Account Payable Report(from webpage)</t>
+  </si>
+  <si>
+    <t>Report Result:
+----------------------Account Payable Report--------------------
+Provider Name: Pizza, Health, and You
+Service Name: 1 On 1 Consultation
+Service fee: 150.00
+Service Name: Self Help Books Lib
+Service fee: 39.99
+Service Name: 1 On 1 Consultation
+Service fee: 150.00
+Service Name: Group Consultation
+Service fee: 50.00
+The sum of fee for this provider: 389.99
+The number of the services: 4
+-------------------------------
+Provider Name: Eat 'Till You Drop
+The sum of fee for this provider: 0
+The number of the services: 0
+-------------------------------
+Provider Name: Pizzario
+The sum of fee for this provider: 0
+The number of the services: 0
+-------------------------------
+Provider Name: Food For Thought
+The sum of fee for this provider: 0
+The number of the services: 0
+-------------------------------
+Provider Name: House of Pizzaholics
+The sum of fee for this provider: 0
+The number of the services: 0
+-------------------------------
+The total fee of all providers: 389.99
+The number of the providers: 5</t>
+  </si>
+  <si>
+    <t>Provider_Eat 'Till You Drop_20_22.txt
+Provider_Food For Thought_20_22.txt
+Provider_House of Pizzaholics_20_22.txt
+Provider_House of Pizzaholics_20_22.txt
+Provider_Pizzario_20_22.txt</t>
+  </si>
+  <si>
+    <t>Member_Aamer Halem_20_13.txt
+Member_Alonzo Bodden_20_13.txt
+Member_Bobcat Goldthwait_20_13.txt
+Member_Brian Babylon_20_13.txt
+Member_Faith Salie_20_13.txt
+Member_Firoozeh Dumas_20_13.txt
+Member_Jessi Klein_20_13.txt
+Member_Luke Burbank_20_13.txt
+Member_Maz Jobrani_20_13.txt
+Member_panshengti_20_13.txt
+Member_Peter Grosz_20_13.txt
+Member_Sue Ellicott_20_13.txt</t>
   </si>
 </sst>
 </file>
@@ -284,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -299,6 +484,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -306,12 +500,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -594,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -605,22 +811,24 @@
     <col min="1" max="1" width="8.7265625" style="3"/>
     <col min="2" max="2" width="35.08984375" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="6" width="26.1796875" customWidth="1"/>
-    <col min="7" max="7" width="26.26953125" customWidth="1"/>
+    <col min="4" max="4" width="32.26953125" customWidth="1"/>
+    <col min="5" max="5" width="36.6328125" customWidth="1"/>
+    <col min="6" max="6" width="34.453125" customWidth="1"/>
+    <col min="7" max="7" width="35.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="7"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -652,16 +860,16 @@
       <c r="C3" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -672,16 +880,16 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -692,13 +900,13 @@
       <c r="C5" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E5" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>49</v>
       </c>
       <c r="G5" t="s">
@@ -715,7 +923,7 @@
       <c r="D6" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>38</v>
       </c>
       <c r="F6" t="s">
@@ -732,143 +940,317 @@
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="10">
+    <row r="8" spans="1:7" ht="232" x14ac:dyDescent="0.35">
+      <c r="B8" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="13">
         <v>1000</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>15</v>
+      <c r="E8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="13">
+        <v>12342</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>11</v>
+      <c r="D9" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="7">
         <v>100</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G11" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="116" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="174" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
         <v>31</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C14" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G14" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
+    <row r="15" spans="1:7" ht="174" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
         <v>27</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C16" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D16" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F16" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
+    <row r="17" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C18" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E18" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F18" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G18" s="6" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D23" s="17"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D24" s="17"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D25" s="17"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="1:7" ht="72.5" customHeight="1" collapsed="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="16"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="16"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="16"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="16"/>
+    </row>
+    <row r="30" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="16"/>
+      <c r="B30" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="13">
+        <v>100</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" s="13">
+        <v>170</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="B39" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="B40" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:G8">
-    <sortState ref="A3:G13">
+    <sortState ref="A3:G18">
       <sortCondition ref="B2:B8"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="2">
+  <mergeCells count="3">
+    <mergeCell ref="A26:A30"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>

</xml_diff>